<commit_message>
app9.py revisando y finalizando
</commit_message>
<xml_diff>
--- a/tmp/a_R3.xlsx
+++ b/tmp/a_R3.xlsx
@@ -4210,7 +4210,7 @@
         <v>116</v>
       </c>
       <c r="G61">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H61">
         <v>24.3</v>
@@ -4228,7 +4228,7 @@
         <v>7751.9</v>
       </c>
       <c r="M61">
-        <v>775190</v>
+        <v>4565869.1</v>
       </c>
       <c r="N61">
         <v>0</v>
@@ -4263,7 +4263,7 @@
         <v>116</v>
       </c>
       <c r="G62">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H62">
         <v>24.3</v>
@@ -4281,10 +4281,10 @@
         <v>7751.9</v>
       </c>
       <c r="M62">
-        <v>720410</v>
+        <v>4243214.9</v>
       </c>
       <c r="N62">
-        <v>4218</v>
+        <v>24844.02</v>
       </c>
       <c r="O62" t="s">
         <v>41</v>
@@ -4316,7 +4316,7 @@
         <v>116</v>
       </c>
       <c r="G63">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -4334,10 +4334,10 @@
         <v>7751.9</v>
       </c>
       <c r="M63">
-        <v>660708</v>
+        <v>3891570.12</v>
       </c>
       <c r="N63">
-        <v>3920</v>
+        <v>23088.8</v>
       </c>
       <c r="O63" t="s">
         <v>41</v>
@@ -4369,7 +4369,7 @@
         <v>116</v>
       </c>
       <c r="G64">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -4387,10 +4387,10 @@
         <v>7751.9</v>
       </c>
       <c r="M64">
-        <v>603503</v>
+        <v>3554632.67</v>
       </c>
       <c r="N64">
-        <v>3517</v>
+        <v>20715.13</v>
       </c>
       <c r="O64" t="s">
         <v>41</v>
@@ -4422,7 +4422,7 @@
         <v>116</v>
       </c>
       <c r="G65">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -4440,10 +4440,10 @@
         <v>7751.9</v>
       </c>
       <c r="M65">
-        <v>548949</v>
+        <v>3233309.61</v>
       </c>
       <c r="N65">
-        <v>3248</v>
+        <v>19130.72</v>
       </c>
       <c r="O65" t="s">
         <v>41</v>
@@ -4475,7 +4475,7 @@
         <v>116</v>
       </c>
       <c r="G66">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -4493,10 +4493,10 @@
         <v>7751.9</v>
       </c>
       <c r="M66">
-        <v>497150</v>
+        <v>2928213.5</v>
       </c>
       <c r="N66">
-        <v>2987</v>
+        <v>17593.43</v>
       </c>
       <c r="O66" t="s">
         <v>41</v>
@@ -4528,7 +4528,7 @@
         <v>116</v>
       </c>
       <c r="G67">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -4546,10 +4546,10 @@
         <v>7751.9</v>
       </c>
       <c r="M67">
-        <v>447651</v>
+        <v>2636664.39</v>
       </c>
       <c r="N67">
-        <v>2705</v>
+        <v>15932.45</v>
       </c>
       <c r="O67" t="s">
         <v>41</v>
@@ -4581,7 +4581,7 @@
         <v>116</v>
       </c>
       <c r="G68">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -4599,10 +4599,10 @@
         <v>7751.9</v>
       </c>
       <c r="M68">
-        <v>400481</v>
+        <v>2358833.09</v>
       </c>
       <c r="N68">
-        <v>2383</v>
+        <v>14035.87</v>
       </c>
       <c r="O68" t="s">
         <v>41</v>
@@ -4634,7 +4634,7 @@
         <v>116</v>
       </c>
       <c r="G69">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -4652,10 +4652,10 @@
         <v>7751.9</v>
       </c>
       <c r="M69">
-        <v>355090</v>
+        <v>2091480.1</v>
       </c>
       <c r="N69">
-        <v>2155</v>
+        <v>12692.95</v>
       </c>
       <c r="O69" t="s">
         <v>41</v>
@@ -4687,7 +4687,7 @@
         <v>116</v>
       </c>
       <c r="G70">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -4705,10 +4705,10 @@
         <v>7751.9</v>
       </c>
       <c r="M70">
-        <v>311509</v>
+        <v>1834788.01</v>
       </c>
       <c r="N70">
-        <v>1932</v>
+        <v>11379.48</v>
       </c>
       <c r="O70" t="s">
         <v>41</v>
@@ -4740,7 +4740,7 @@
         <v>116</v>
       </c>
       <c r="G71">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -4758,10 +4758,10 @@
         <v>7751.9</v>
       </c>
       <c r="M71">
-        <v>269514</v>
+        <v>1587437.46</v>
       </c>
       <c r="N71">
-        <v>1695</v>
+        <v>9983.549999999999</v>
       </c>
       <c r="O71" t="s">
         <v>41</v>
@@ -4793,7 +4793,7 @@
         <v>116</v>
       </c>
       <c r="G72">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4811,10 +4811,10 @@
         <v>7751.9</v>
       </c>
       <c r="M72">
-        <v>229243</v>
+        <v>1350241.27</v>
       </c>
       <c r="N72">
-        <v>1450</v>
+        <v>8540.5</v>
       </c>
       <c r="O72" t="s">
         <v>41</v>
@@ -4846,7 +4846,7 @@
         <v>116</v>
       </c>
       <c r="G73">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -4864,10 +4864,10 @@
         <v>7751.9</v>
       </c>
       <c r="M73">
-        <v>190495</v>
+        <v>1122015.55</v>
       </c>
       <c r="N73">
-        <v>1234</v>
+        <v>7268.26</v>
       </c>
       <c r="O73" t="s">
         <v>41</v>
@@ -4899,7 +4899,7 @@
         <v>116</v>
       </c>
       <c r="G74">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -4917,10 +4917,10 @@
         <v>7751.9</v>
       </c>
       <c r="M74">
-        <v>153302</v>
+        <v>902948.78</v>
       </c>
       <c r="N74">
-        <v>1059</v>
+        <v>6237.51</v>
       </c>
       <c r="O74" t="s">
         <v>41</v>
@@ -4952,7 +4952,7 @@
         <v>116</v>
       </c>
       <c r="G75">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -4970,10 +4970,10 @@
         <v>7751.9</v>
       </c>
       <c r="M75">
-        <v>117592</v>
+        <v>692616.88</v>
       </c>
       <c r="N75">
-        <v>825</v>
+        <v>4859.25</v>
       </c>
       <c r="O75" t="s">
         <v>41</v>
@@ -5005,7 +5005,7 @@
         <v>116</v>
       </c>
       <c r="G76">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -5023,10 +5023,10 @@
         <v>7751.9</v>
       </c>
       <c r="M76">
-        <v>83283</v>
+        <v>490536.87</v>
       </c>
       <c r="N76">
-        <v>633</v>
+        <v>3728.37</v>
       </c>
       <c r="O76" t="s">
         <v>41</v>
@@ -5058,7 +5058,7 @@
         <v>116</v>
       </c>
       <c r="G77">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -5076,10 +5076,10 @@
         <v>7751.9</v>
       </c>
       <c r="M77">
-        <v>50326</v>
+        <v>296420.14</v>
       </c>
       <c r="N77">
-        <v>448</v>
+        <v>2638.72</v>
       </c>
       <c r="O77" t="s">
         <v>41</v>
@@ -5111,7 +5111,7 @@
         <v>116</v>
       </c>
       <c r="G78">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -5129,10 +5129,10 @@
         <v>7751.9</v>
       </c>
       <c r="M78">
-        <v>18671</v>
+        <v>109972.19</v>
       </c>
       <c r="N78">
-        <v>271</v>
+        <v>1596.19</v>
       </c>
       <c r="O78" t="s">
         <v>41</v>
@@ -5164,7 +5164,7 @@
         <v>116</v>
       </c>
       <c r="G79">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -5185,7 +5185,7 @@
         <v>0</v>
       </c>
       <c r="N79">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="O79" t="s">
         <v>41</v>
@@ -5217,7 +5217,7 @@
         <v>116</v>
       </c>
       <c r="G80">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H80">
         <v>24.3</v>
@@ -5235,7 +5235,7 @@
         <v>7751.9</v>
       </c>
       <c r="M80">
-        <v>775190</v>
+        <v>4565869.1</v>
       </c>
       <c r="N80">
         <v>0</v>
@@ -5270,7 +5270,7 @@
         <v>116</v>
       </c>
       <c r="G81">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H81">
         <v>24.3</v>
@@ -5288,10 +5288,10 @@
         <v>7751.9</v>
       </c>
       <c r="M81">
-        <v>724551</v>
+        <v>4267605.39</v>
       </c>
       <c r="N81">
-        <v>4218</v>
+        <v>24844.02</v>
       </c>
       <c r="O81" t="s">
         <v>45</v>
@@ -5323,7 +5323,7 @@
         <v>116</v>
       </c>
       <c r="G82">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -5341,10 +5341,10 @@
         <v>7751.9</v>
       </c>
       <c r="M82">
-        <v>676571</v>
+        <v>3985003.19</v>
       </c>
       <c r="N82">
-        <v>3942</v>
+        <v>23218.38</v>
       </c>
       <c r="O82" t="s">
         <v>45</v>
@@ -5376,7 +5376,7 @@
         <v>116</v>
       </c>
       <c r="G83">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -5394,10 +5394,10 @@
         <v>7751.9</v>
       </c>
       <c r="M83">
-        <v>630079</v>
+        <v>3711165.31</v>
       </c>
       <c r="N83">
-        <v>3601</v>
+        <v>21209.89</v>
       </c>
       <c r="O83" t="s">
         <v>45</v>
@@ -5429,7 +5429,7 @@
         <v>116</v>
       </c>
       <c r="G84">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -5447,10 +5447,10 @@
         <v>7751.9</v>
       </c>
       <c r="M84">
-        <v>585295</v>
+        <v>3447387.55</v>
       </c>
       <c r="N84">
-        <v>3391</v>
+        <v>19972.99</v>
       </c>
       <c r="O84" t="s">
         <v>45</v>
@@ -5482,7 +5482,7 @@
         <v>116</v>
       </c>
       <c r="G85">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -5500,10 +5500,10 @@
         <v>7751.9</v>
       </c>
       <c r="M85">
-        <v>542391</v>
+        <v>3194682.99</v>
       </c>
       <c r="N85">
-        <v>3184</v>
+        <v>18753.76</v>
       </c>
       <c r="O85" t="s">
         <v>45</v>
@@ -5535,7 +5535,7 @@
         <v>116</v>
       </c>
       <c r="G86">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -5553,10 +5553,10 @@
         <v>7751.9</v>
       </c>
       <c r="M86">
-        <v>500957</v>
+        <v>2950636.73</v>
       </c>
       <c r="N86">
-        <v>2951</v>
+        <v>17381.39</v>
       </c>
       <c r="O86" t="s">
         <v>45</v>
@@ -5588,7 +5588,7 @@
         <v>116</v>
       </c>
       <c r="G87">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -5606,10 +5606,10 @@
         <v>7751.9</v>
       </c>
       <c r="M87">
-        <v>461082</v>
+        <v>2715772.98</v>
       </c>
       <c r="N87">
-        <v>2666</v>
+        <v>15702.74</v>
       </c>
       <c r="O87" t="s">
         <v>45</v>
@@ -5641,7 +5641,7 @@
         <v>116</v>
       </c>
       <c r="G88">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -5659,10 +5659,10 @@
         <v>7751.9</v>
       </c>
       <c r="M88">
-        <v>422234</v>
+        <v>2486958.26</v>
       </c>
       <c r="N88">
-        <v>2481</v>
+        <v>14613.09</v>
       </c>
       <c r="O88" t="s">
         <v>45</v>
@@ -5694,7 +5694,7 @@
         <v>116</v>
       </c>
       <c r="G89">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -5712,10 +5712,10 @@
         <v>7751.9</v>
       </c>
       <c r="M89">
-        <v>384488</v>
+        <v>2264634.32</v>
       </c>
       <c r="N89">
-        <v>2297</v>
+        <v>13529.33</v>
       </c>
       <c r="O89" t="s">
         <v>45</v>
@@ -5747,7 +5747,7 @@
         <v>116</v>
       </c>
       <c r="G90">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H90">
         <v>0</v>
@@ -5765,10 +5765,10 @@
         <v>7751.9</v>
       </c>
       <c r="M90">
-        <v>347645</v>
+        <v>2047629.05</v>
       </c>
       <c r="N90">
-        <v>2092</v>
+        <v>12321.88</v>
       </c>
       <c r="O90" t="s">
         <v>45</v>
@@ -5800,7 +5800,7 @@
         <v>116</v>
       </c>
       <c r="G91">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H91">
         <v>0</v>
@@ -5818,10 +5818,10 @@
         <v>7751.9</v>
       </c>
       <c r="M91">
-        <v>311894</v>
+        <v>1837055.66</v>
       </c>
       <c r="N91">
-        <v>1871</v>
+        <v>11020.19</v>
       </c>
       <c r="O91" t="s">
         <v>45</v>
@@ -5853,7 +5853,7 @@
         <v>116</v>
       </c>
       <c r="G92">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -5871,10 +5871,10 @@
         <v>7751.9</v>
       </c>
       <c r="M92">
-        <v>277057</v>
+        <v>1631865.73</v>
       </c>
       <c r="N92">
-        <v>1679</v>
+        <v>9889.309999999999</v>
       </c>
       <c r="O92" t="s">
         <v>45</v>
@@ -5906,7 +5906,7 @@
         <v>116</v>
       </c>
       <c r="G93">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -5924,10 +5924,10 @@
         <v>7751.9</v>
       </c>
       <c r="M93">
-        <v>243206</v>
+        <v>1432483.34</v>
       </c>
       <c r="N93">
-        <v>1540</v>
+        <v>9070.6</v>
       </c>
       <c r="O93" t="s">
         <v>45</v>
@@ -5959,7 +5959,7 @@
         <v>116</v>
       </c>
       <c r="G94">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -5977,10 +5977,10 @@
         <v>7751.9</v>
       </c>
       <c r="M94">
-        <v>210299</v>
+        <v>1238661.11</v>
       </c>
       <c r="N94">
-        <v>1309</v>
+        <v>7710.01</v>
       </c>
       <c r="O94" t="s">
         <v>45</v>
@@ -6012,7 +6012,7 @@
         <v>116</v>
       </c>
       <c r="G95">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -6030,10 +6030,10 @@
         <v>7751.9</v>
       </c>
       <c r="M95">
-        <v>178282</v>
+        <v>1050080.98</v>
       </c>
       <c r="N95">
-        <v>1132</v>
+        <v>6667.48</v>
       </c>
       <c r="O95" t="s">
         <v>45</v>
@@ -6065,7 +6065,7 @@
         <v>116</v>
       </c>
       <c r="G96">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -6083,10 +6083,10 @@
         <v>7751.9</v>
       </c>
       <c r="M96">
-        <v>147132</v>
+        <v>866607.48</v>
       </c>
       <c r="N96">
-        <v>959</v>
+        <v>5648.51</v>
       </c>
       <c r="O96" t="s">
         <v>45</v>
@@ -6118,7 +6118,7 @@
         <v>116</v>
       </c>
       <c r="G97">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -6136,10 +6136,10 @@
         <v>7751.9</v>
       </c>
       <c r="M97">
-        <v>116828</v>
+        <v>688116.92</v>
       </c>
       <c r="N97">
-        <v>792</v>
+        <v>4664.88</v>
       </c>
       <c r="O97" t="s">
         <v>45</v>
@@ -6171,7 +6171,7 @@
         <v>116</v>
       </c>
       <c r="G98">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -6189,10 +6189,10 @@
         <v>7751.9</v>
       </c>
       <c r="M98">
-        <v>87357</v>
+        <v>514532.73</v>
       </c>
       <c r="N98">
-        <v>629</v>
+        <v>3704.81</v>
       </c>
       <c r="O98" t="s">
         <v>45</v>
@@ -6224,7 +6224,7 @@
         <v>116</v>
       </c>
       <c r="G99">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -6242,10 +6242,10 @@
         <v>7751.9</v>
       </c>
       <c r="M99">
-        <v>58679</v>
+        <v>345619.31</v>
       </c>
       <c r="N99">
-        <v>470</v>
+        <v>2768.3</v>
       </c>
       <c r="O99" t="s">
         <v>45</v>
@@ -6277,7 +6277,7 @@
         <v>116</v>
       </c>
       <c r="G100">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H100">
         <v>0</v>
@@ -6295,10 +6295,10 @@
         <v>7751.9</v>
       </c>
       <c r="M100">
-        <v>30809</v>
+        <v>181465.01</v>
       </c>
       <c r="N100">
-        <v>316</v>
+        <v>1861.24</v>
       </c>
       <c r="O100" t="s">
         <v>45</v>
@@ -6330,7 +6330,7 @@
         <v>116</v>
       </c>
       <c r="G101">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -6348,10 +6348,10 @@
         <v>7751.9</v>
       </c>
       <c r="M101">
-        <v>3777</v>
+        <v>22246.53</v>
       </c>
       <c r="N101">
-        <v>166</v>
+        <v>977.74</v>
       </c>
       <c r="O101" t="s">
         <v>45</v>
@@ -6383,7 +6383,7 @@
         <v>116</v>
       </c>
       <c r="G102">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -6404,7 +6404,7 @@
         <v>-0</v>
       </c>
       <c r="N102">
-        <v>21</v>
+        <v>123.69</v>
       </c>
       <c r="O102" t="s">
         <v>45</v>
@@ -6436,7 +6436,7 @@
         <v>116</v>
       </c>
       <c r="G103">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H103">
         <v>24.3</v>
@@ -6454,7 +6454,7 @@
         <v>7751.9</v>
       </c>
       <c r="M103">
-        <v>775190</v>
+        <v>4565869.1</v>
       </c>
       <c r="N103">
         <v>0</v>
@@ -6489,7 +6489,7 @@
         <v>116</v>
       </c>
       <c r="G104">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H104">
         <v>24.3</v>
@@ -6507,10 +6507,10 @@
         <v>7751.9</v>
       </c>
       <c r="M104">
-        <v>716832</v>
+        <v>4222140.48</v>
       </c>
       <c r="N104">
-        <v>4218</v>
+        <v>24844.02</v>
       </c>
       <c r="O104" t="s">
         <v>39</v>
@@ -6542,7 +6542,7 @@
         <v>116</v>
       </c>
       <c r="G105">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -6560,10 +6560,10 @@
         <v>7751.9</v>
       </c>
       <c r="M105">
-        <v>647126</v>
+        <v>3811572.14</v>
       </c>
       <c r="N105">
-        <v>3900</v>
+        <v>22971</v>
       </c>
       <c r="O105" t="s">
         <v>39</v>
@@ -6595,7 +6595,7 @@
         <v>116</v>
       </c>
       <c r="G106">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H106">
         <v>0</v>
@@ -6613,10 +6613,10 @@
         <v>7751.9</v>
       </c>
       <c r="M106">
-        <v>580954</v>
+        <v>3421819.06</v>
       </c>
       <c r="N106">
-        <v>3444</v>
+        <v>20285.16</v>
       </c>
       <c r="O106" t="s">
         <v>39</v>
@@ -6648,7 +6648,7 @@
         <v>116</v>
       </c>
       <c r="G107">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H107">
         <v>0</v>
@@ -6666,10 +6666,10 @@
         <v>7751.9</v>
       </c>
       <c r="M107">
-        <v>518391</v>
+        <v>3053322.99</v>
       </c>
       <c r="N107">
-        <v>3126</v>
+        <v>18412.14</v>
       </c>
       <c r="O107" t="s">
         <v>39</v>
@@ -6701,7 +6701,7 @@
         <v>116</v>
       </c>
       <c r="G108">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H108">
         <v>0</v>
@@ -6719,10 +6719,10 @@
         <v>7751.9</v>
       </c>
       <c r="M108">
-        <v>459459</v>
+        <v>2706213.51</v>
       </c>
       <c r="N108">
-        <v>2820</v>
+        <v>16609.8</v>
       </c>
       <c r="O108" t="s">
         <v>39</v>
@@ -6754,7 +6754,7 @@
         <v>116</v>
       </c>
       <c r="G109">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H109">
         <v>0</v>
@@ -6772,10 +6772,10 @@
         <v>7751.9</v>
       </c>
       <c r="M109">
-        <v>403644</v>
+        <v>2377463.16</v>
       </c>
       <c r="N109">
-        <v>2500</v>
+        <v>14725</v>
       </c>
       <c r="O109" t="s">
         <v>39</v>
@@ -6807,7 +6807,7 @@
         <v>116</v>
       </c>
       <c r="G110">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H110">
         <v>0</v>
@@ -6825,10 +6825,10 @@
         <v>7751.9</v>
       </c>
       <c r="M110">
-        <v>350907</v>
+        <v>2066842.23</v>
       </c>
       <c r="N110">
-        <v>2148</v>
+        <v>12651.72</v>
       </c>
       <c r="O110" t="s">
         <v>39</v>
@@ -6860,7 +6860,7 @@
         <v>116</v>
       </c>
       <c r="G111">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H111">
         <v>0</v>
@@ -6878,10 +6878,10 @@
         <v>7751.9</v>
       </c>
       <c r="M111">
-        <v>300664</v>
+        <v>1770910.96</v>
       </c>
       <c r="N111">
-        <v>1888</v>
+        <v>11120.32</v>
       </c>
       <c r="O111" t="s">
         <v>39</v>
@@ -6913,7 +6913,7 @@
         <v>116</v>
       </c>
       <c r="G112">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H112">
         <v>0</v>
@@ -6931,10 +6931,10 @@
         <v>7751.9</v>
       </c>
       <c r="M112">
-        <v>252891</v>
+        <v>1489527.99</v>
       </c>
       <c r="N112">
-        <v>1636</v>
+        <v>9636.040000000001</v>
       </c>
       <c r="O112" t="s">
         <v>39</v>
@@ -6966,7 +6966,7 @@
         <v>116</v>
       </c>
       <c r="G113">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H113">
         <v>0</v>
@@ -6984,10 +6984,10 @@
         <v>7751.9</v>
       </c>
       <c r="M113">
-        <v>207330</v>
+        <v>1221173.7</v>
       </c>
       <c r="N113">
-        <v>1376</v>
+        <v>8104.64</v>
       </c>
       <c r="O113" t="s">
         <v>39</v>
@@ -7019,7 +7019,7 @@
         <v>116</v>
       </c>
       <c r="G114">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H114">
         <v>0</v>
@@ -7037,10 +7037,10 @@
         <v>7751.9</v>
       </c>
       <c r="M114">
-        <v>164060</v>
+        <v>966313.4</v>
       </c>
       <c r="N114">
-        <v>1116</v>
+        <v>6573.24</v>
       </c>
       <c r="O114" t="s">
         <v>39</v>
@@ -7072,7 +7072,7 @@
         <v>116</v>
       </c>
       <c r="G115">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H115">
         <v>0</v>
@@ -7090,10 +7090,10 @@
         <v>7751.9</v>
       </c>
       <c r="M115">
-        <v>122850</v>
+        <v>723586.5</v>
       </c>
       <c r="N115">
-        <v>883</v>
+        <v>5200.87</v>
       </c>
       <c r="O115" t="s">
         <v>39</v>
@@ -7125,7 +7125,7 @@
         <v>116</v>
       </c>
       <c r="G116">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H116">
         <v>0</v>
@@ -7143,10 +7143,10 @@
         <v>7751.9</v>
       </c>
       <c r="M116">
-        <v>83686</v>
+        <v>492910.54</v>
       </c>
       <c r="N116">
-        <v>683</v>
+        <v>4022.87</v>
       </c>
       <c r="O116" t="s">
         <v>39</v>
@@ -7178,7 +7178,7 @@
         <v>116</v>
       </c>
       <c r="G117">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H117">
         <v>0</v>
@@ -7196,10 +7196,10 @@
         <v>7751.9</v>
       </c>
       <c r="M117">
-        <v>46459</v>
+        <v>273643.51</v>
       </c>
       <c r="N117">
-        <v>450</v>
+        <v>2650.5</v>
       </c>
       <c r="O117" t="s">
         <v>39</v>
@@ -7231,7 +7231,7 @@
         <v>116</v>
       </c>
       <c r="G118">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H118">
         <v>0</v>
@@ -7249,10 +7249,10 @@
         <v>7751.9</v>
       </c>
       <c r="M118">
-        <v>11056</v>
+        <v>65119.84</v>
       </c>
       <c r="N118">
-        <v>250</v>
+        <v>1472.5</v>
       </c>
       <c r="O118" t="s">
         <v>39</v>
@@ -7284,7 +7284,7 @@
         <v>116</v>
       </c>
       <c r="G119">
-        <v>100</v>
+        <v>589</v>
       </c>
       <c r="H119">
         <v>0</v>
@@ -7302,10 +7302,10 @@
         <v>7751.9</v>
       </c>
       <c r="M119">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="N119">
-        <v>59</v>
+        <v>347.51</v>
       </c>
       <c r="O119" t="s">
         <v>39</v>

</xml_diff>